<commit_message>
Updated Timeline and Requirement Document
</commit_message>
<xml_diff>
--- a/docs/Timeline.xlsx
+++ b/docs/Timeline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Activity</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Library chosen: EmguCV (OpenCV wrapper for C# .NET)</t>
-  </si>
-  <si>
-    <t>Currently in Progress</t>
   </si>
 </sst>
 </file>
@@ -444,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,8 +569,8 @@
       <c r="E6" s="2">
         <v>43012</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
+      <c r="F6" s="2">
+        <v>43014</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -588,6 +585,9 @@
       </c>
       <c r="D7" s="2">
         <v>43016</v>
+      </c>
+      <c r="E7" s="2">
+        <v>43014</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes (Top Level): - Finished Face Recognition Engine - Initial development on form app client
</commit_message>
<xml_diff>
--- a/docs/Timeline.xlsx
+++ b/docs/Timeline.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
+    <sheet name="Development Module Breakdown" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Activity</t>
   </si>
@@ -102,6 +103,36 @@
   </si>
   <si>
     <t>Library chosen: EmguCV (OpenCV wrapper for C# .NET)</t>
+  </si>
+  <si>
+    <t>Switch Priority to project structure</t>
+  </si>
+  <si>
+    <t>Stuck on troubleshoot using the library</t>
+  </si>
+  <si>
+    <t>Start Unit Test after development finished (Each module)</t>
+  </si>
+  <si>
+    <t>Module Part</t>
+  </si>
+  <si>
+    <t>Encryption</t>
+  </si>
+  <si>
+    <t>I/O Manager</t>
+  </si>
+  <si>
+    <t>Setting Management</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
   </si>
 </sst>
 </file>
@@ -145,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +184,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,27 +491,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -490,7 +524,7 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -589,6 +623,12 @@
       <c r="E7" s="2">
         <v>43014</v>
       </c>
+      <c r="F7" s="2">
+        <v>43023</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -603,7 +643,9 @@
       <c r="D8" s="3">
         <v>43043</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="3">
+        <v>43014</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -619,6 +661,12 @@
       <c r="D9" s="2">
         <v>43016</v>
       </c>
+      <c r="E9" s="2">
+        <v>43014</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43014</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -633,6 +681,15 @@
       <c r="D10" s="2">
         <v>43017</v>
       </c>
+      <c r="E10" s="2">
+        <v>43014</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43023</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -647,6 +704,12 @@
       <c r="D11" s="2">
         <v>43018</v>
       </c>
+      <c r="E11" s="2">
+        <v>43023</v>
+      </c>
+      <c r="F11" s="2">
+        <v>43023</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -701,6 +764,12 @@
       </c>
       <c r="D16" s="2">
         <v>43041</v>
+      </c>
+      <c r="E16" s="2">
+        <v>43023</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -725,4 +794,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43023</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43023</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43023</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>